<commit_message>
Izzy worked on dissertation
</commit_message>
<xml_diff>
--- a/data/error_accuracy_documentation.xlsx
+++ b/data/error_accuracy_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/izzyrich/Documents/Edinburgh Year 4/dissertation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A09747-E279-1B4D-B5C3-499CF957307A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFFCC5B-BEB6-694C-9C3B-1525EE464DF3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="1760" windowWidth="26740" windowHeight="14420" xr2:uid="{FCD01B9E-DE46-7646-A223-7A649FFB08E1}"/>
+    <workbookView xWindow="580" yWindow="940" windowWidth="26740" windowHeight="14420" xr2:uid="{FCD01B9E-DE46-7646-A223-7A649FFB08E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>